<commit_message>
Fixed NewSell to Work on Template but Still needs frontend
</commit_message>
<xml_diff>
--- a/proyecto_db/test.xlsx
+++ b/proyecto_db/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNI\Proyect DB\DB_Proyect\proyecto_db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB64E555-5C15-4C5E-B414-E14A8C1902D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18016366-1D96-4CC1-8886-46B158366E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Nombre</t>
   </si>
@@ -36,7 +36,10 @@
     <t>Cantidad</t>
   </si>
   <si>
-    <t>Lapiz Grafito</t>
+    <t>Cuaderno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Libreta </t>
   </si>
 </sst>
 </file>
@@ -354,15 +357,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -373,15 +376,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>